<commit_message>
updated the part numbers and such
</commit_message>
<xml_diff>
--- a/Manufacturing/JD Laser Order 222/WR Tube Request 2022.xlsx
+++ b/Manufacturing/JD Laser Order 222/WR Tube Request 2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajkof\Documents\Wisconsin Racing\git\CAD\active-cad\Manufacturing\JD Laser Order 222\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Desktop\`\GitHub\active-cad\Manufacturing\JD Laser Order 222\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3D854F-1F4D-4115-B487-6AEF71B958A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6505465D-523A-4C3A-9F5A-7BB86691CDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17256" yWindow="1944" windowWidth="7500" windowHeight="6000" xr2:uid="{5EEE3E8E-3ADA-4319-A780-7D4EFF66DEBB}"/>
+    <workbookView xWindow="28680" yWindow="-8850" windowWidth="29040" windowHeight="16440" xr2:uid="{5EEE3E8E-3ADA-4319-A780-7D4EFF66DEBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Part Number</t>
   </si>
@@ -96,7 +96,16 @@
     <t>8-foot length of uncut tube if available</t>
   </si>
   <si>
-    <t>280-XX-22-A</t>
+    <t>280-011-22-A</t>
+  </si>
+  <si>
+    <t>280-013-22-A</t>
+  </si>
+  <si>
+    <t>280-014-22-A</t>
+  </si>
+  <si>
+    <t>280-015-22-A</t>
   </si>
 </sst>
 </file>
@@ -453,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45ED9460-79D1-4A1B-AE35-96457925AC81}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,42 +667,89 @@
       <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>9.5000000000000001E-2</v>
+      </c>
       <c r="D14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="1">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>3.5000000000000003E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>